<commit_message>
Slight change to explicit list
Moved keyword "abuse" from explicit to implicit. Makes more sense in context.
</commit_message>
<xml_diff>
--- a/server/trainingSets/explicit.xlsx
+++ b/server/trainingSets/explicit.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manukastratta/Box Sync/STANFORD/courses/COURSES/FALL-2019/CS197/project/DeText/trainingSets/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/manukastratta/Box Sync/STANFORD/courses/COURSES/FALL-2019/CS197/197_extensions/DeText/server/trainingSets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A92997E2-68F0-6A4F-A495-92A688F55497}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26998B72-938D-7340-ABE9-6ECC5E8C01B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1420" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Explicit" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>date rape</t>
-  </si>
-  <si>
-    <t>abuse</t>
   </si>
   <si>
     <t>daterape</t>
@@ -435,7 +432,7 @@
   <dimension ref="A1:Z1385"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -446,7 +443,7 @@
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="16" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -473,8 +470,8 @@
       <c r="Z1" s="3"/>
     </row>
     <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="16" t="s">
-        <v>3</v>
+      <c r="A2" s="14" t="s">
+        <v>0</v>
       </c>
       <c r="D2" s="5"/>
       <c r="G2" s="6"/>
@@ -500,7 +497,7 @@
     </row>
     <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D3" s="5"/>
       <c r="F3" s="6"/>
@@ -526,8 +523,8 @@
       <c r="Z3" s="6"/>
     </row>
     <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="14" t="s">
-        <v>2</v>
+      <c r="A4" s="15" t="s">
+        <v>17</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6"/>
@@ -554,8 +551,8 @@
       <c r="Z4" s="6"/>
     </row>
     <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="15" t="s">
-        <v>18</v>
+      <c r="A5" s="14" t="s">
+        <v>3</v>
       </c>
       <c r="C5" s="8"/>
       <c r="D5" s="6"/>
@@ -584,7 +581,7 @@
     </row>
     <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C6" s="8"/>
       <c r="D6" s="6"/>
@@ -613,7 +610,7 @@
     </row>
     <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
       <c r="C7" s="8"/>
       <c r="D7" s="6"/>
@@ -642,7 +639,7 @@
     </row>
     <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="C8" s="8"/>
       <c r="D8" s="6"/>
@@ -700,7 +697,7 @@
     </row>
     <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C10" s="8"/>
       <c r="D10" s="6"/>
@@ -729,7 +726,7 @@
     </row>
     <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="C11" s="8"/>
       <c r="D11" s="6"/>
@@ -787,7 +784,7 @@
     </row>
     <row r="13" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="14" t="s">
-        <v>12</v>
+        <v>4</v>
       </c>
       <c r="C13" s="8"/>
       <c r="D13" s="6"/>
@@ -816,7 +813,7 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="14" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C14" s="8"/>
       <c r="D14" s="6"/>
@@ -845,7 +842,7 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="14" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C15" s="8"/>
       <c r="D15" s="6"/>
@@ -874,7 +871,7 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="C16" s="8"/>
       <c r="D16" s="6"/>
@@ -903,7 +900,7 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="14" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C17" s="8"/>
       <c r="D17" s="6"/>
@@ -932,7 +929,7 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="14" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C18" s="8"/>
       <c r="D18" s="6"/>
@@ -961,7 +958,7 @@
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="14" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="6"/>
@@ -989,8 +986,8 @@
       <c r="Z19" s="6"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="14" t="s">
-        <v>6</v>
+      <c r="A20" s="15" t="s">
+        <v>18</v>
       </c>
       <c r="C20" s="7"/>
       <c r="D20" s="6"/>
@@ -1019,7 +1016,7 @@
     </row>
     <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C21" s="7"/>
       <c r="D21" s="6"/>
@@ -1047,8 +1044,8 @@
       <c r="Z21" s="6"/>
     </row>
     <row r="22" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A22" s="15" t="s">
-        <v>21</v>
+      <c r="A22" t="s">
+        <v>16</v>
       </c>
       <c r="C22" s="7"/>
       <c r="D22" s="6"/>
@@ -1076,8 +1073,8 @@
       <c r="Z22" s="6"/>
     </row>
     <row r="23" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" t="s">
-        <v>17</v>
+      <c r="A23" s="6" t="s">
+        <v>23</v>
       </c>
       <c r="B23" s="4"/>
       <c r="D23" s="6"/>
@@ -1106,7 +1103,7 @@
     </row>
     <row r="24" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A24" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="4"/>
       <c r="D24" s="6"/>
@@ -1135,7 +1132,7 @@
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A25" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="4"/>
       <c r="D25" s="6"/>
@@ -1164,7 +1161,7 @@
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
@@ -1193,9 +1190,7 @@
       <c r="Z26" s="6"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="6" t="s">
-        <v>24</v>
-      </c>
+      <c r="A27" s="16"/>
       <c r="B27" s="6"/>
       <c r="D27" s="6"/>
       <c r="E27" s="6"/>

</xml_diff>